<commit_message>
Updated isotope. standards dataset to include VSMOW relative to air
</commit_message>
<xml_diff>
--- a/data-raw/isotope.standards.xlsx
+++ b/data-raw/isotope.standards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwh/Dropbox/Documents/RPackages/HEEL/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09658C74-009D-1447-A418-931224B6B353}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A67D4F0-12F2-8A49-BCB6-0774B529C756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="4540" windowWidth="45380" windowHeight="17440" xr2:uid="{BC01E585-F9B4-1C40-8E70-833A08362EF2}"/>
+    <workbookView xWindow="0" yWindow="1960" windowWidth="33600" windowHeight="17440" xr2:uid="{BC01E585-F9B4-1C40-8E70-833A08362EF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -265,9 +265,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -309,13 +311,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +640,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -733,7 +740,7 @@
       <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="6">
         <v>1.1180000000000001E-2</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -789,17 +796,17 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <f>1/272</f>
         <v>3.6764705882352941E-3</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="7">
         <v>75.52</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -814,11 +821,12 @@
       <c r="M3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>22</v>
+      <c r="N3">
+        <v>23.8</v>
+      </c>
+      <c r="O3" s="5">
+        <f>$O$4*(N3/1000+1)</f>
+        <v>2.0528941764033338E-3</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>22</v>
@@ -826,7 +834,7 @@
       <c r="Q3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="7">
         <v>23.14</v>
       </c>
       <c r="S3" s="1" t="s">
@@ -858,13 +866,13 @@
       <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -882,24 +890,24 @@
       <c r="N4" s="1">
         <v>0</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="8">
         <f>0.0020004/0.9976206</f>
         <v>2.0051711041251551E-3</v>
       </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
         <f>0.000379/0.9976206</f>
         <v>3.7990394344302836E-4</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="10">
         <f>0.00015574/0.99984426</f>
         <v>1.5576425872565393E-4</v>
       </c>
@@ -926,13 +934,13 @@
       <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -941,7 +949,7 @@
       <c r="K5" s="1">
         <v>0</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="9">
         <v>4.3992910000000003E-2</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -950,7 +958,7 @@
       <c r="N5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -959,13 +967,13 @@
       <c r="Q5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U5" s="1" t="s">
@@ -988,17 +996,17 @@
       <c r="E6" s="1">
         <v>180</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <f>$F$3*(E6/1000+1)</f>
         <v>4.3382352941176471E-3</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="7">
         <v>16.48</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -1016,7 +1024,7 @@
       <c r="N6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -1025,13 +1033,13 @@
       <c r="Q6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="7">
         <v>56.472000000000001</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U6" s="1" t="s">
@@ -1054,21 +1062,21 @@
       <c r="E7" s="1">
         <v>-4.5199999999999996</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="5">
         <f t="shared" ref="F7:F8" si="0">$F$3*(E7/1000+1)</f>
         <v>3.6598529411764709E-3</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="7">
         <v>9.52</v>
       </c>
       <c r="H7" s="1">
         <v>-26.39</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="6">
         <f>$I$2*(H7/1000+1)</f>
         <v>1.08849598E-2</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <v>40.817</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1083,7 +1091,7 @@
       <c r="N7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -1092,13 +1100,13 @@
       <c r="Q7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U7" s="1" t="s">
@@ -1121,21 +1129,21 @@
       <c r="E8" s="1">
         <v>47.57</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>3.8513602941176468E-3</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="7">
         <v>9.52</v>
       </c>
       <c r="H8" s="1">
         <v>37.630000000000003</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="6">
         <f t="shared" ref="I8:I51" si="1">$I$2*(H8/1000+1)</f>
         <v>1.1600703400000001E-2</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>40.817</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1150,7 +1158,7 @@
       <c r="N8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -1159,13 +1167,13 @@
       <c r="Q8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U8" s="1" t="s">
@@ -1188,20 +1196,20 @@
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="1">
         <v>-32.15</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="6">
         <f t="shared" si="1"/>
         <v>1.0820563E-2</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>42.106000000000002</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1216,7 +1224,7 @@
       <c r="N9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -1225,16 +1233,16 @@
       <c r="Q9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="7">
         <v>51.414999999999999</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U9" s="1">
+      <c r="T9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U9" s="3">
         <v>6.4779999999999998</v>
       </c>
     </row>
@@ -1254,20 +1262,20 @@
       <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="1">
         <v>-10.45</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="6">
         <f t="shared" si="1"/>
         <v>1.1063169000000001E-2</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>42.106000000000002</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1282,7 +1290,7 @@
       <c r="N10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -1291,16 +1299,16 @@
       <c r="Q10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="7">
         <v>51.414999999999999</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U10" s="1">
+      <c r="T10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" s="3">
         <v>6.4779999999999998</v>
       </c>
     </row>
@@ -1320,21 +1328,21 @@
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="5">
         <f t="shared" ref="F11" si="2">$F$3*(E11/1000+1)</f>
         <v>3.6838235294117646E-3</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="7">
         <v>2.9649999999999999</v>
       </c>
       <c r="H11" s="1">
         <v>-26.1</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="6">
         <f t="shared" si="1"/>
         <v>1.0888202000000001E-2</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="3">
         <v>45.5</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -1343,13 +1351,13 @@
       <c r="L11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="2">
         <v>0.2</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P11" s="1" t="s">
@@ -1358,16 +1366,16 @@
       <c r="Q11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U11" s="1" t="s">
+      <c r="T11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U11" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1387,19 +1395,19 @@
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="1">
         <v>1.95</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="6">
         <v>1.12021E-2</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>12</v>
       </c>
       <c r="K12" s="1" t="s">
@@ -1414,7 +1422,7 @@
       <c r="N12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P12" s="1" t="s">
@@ -1423,16 +1431,16 @@
       <c r="Q12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="7">
         <v>47.957000000000001</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U12" s="1" t="s">
+      <c r="T12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1452,20 +1460,20 @@
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="1">
         <v>-46.6</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="6">
         <f t="shared" si="1"/>
         <v>1.0659012000000001E-2</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
         <v>16.254999999999999</v>
       </c>
       <c r="K13" s="1" t="s">
@@ -1480,7 +1488,7 @@
       <c r="N13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P13" s="1" t="s">
@@ -1489,16 +1497,16 @@
       <c r="Q13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R13" s="1">
+      <c r="R13" s="7">
         <v>64.957999999999998</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U13" s="1" t="s">
+      <c r="T13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1518,21 +1526,21 @@
       <c r="E14" s="1">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="5">
         <f t="shared" ref="F14:F34" si="3">$F$3*(E14/1000+1)</f>
         <v>3.6595588235294116E-3</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="7">
         <v>9.52</v>
       </c>
       <c r="H14" s="1">
         <v>-28.3</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="6">
         <f t="shared" si="1"/>
         <v>1.0863606000000001E-2</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="3">
         <v>40.817</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -1547,7 +1555,7 @@
       <c r="N14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="O14" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P14" s="1" t="s">
@@ -1556,16 +1564,16 @@
       <c r="Q14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="R14" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U14" s="1" t="s">
+      <c r="T14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1585,21 +1593,21 @@
       <c r="E15" s="1">
         <v>-5.2</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="5">
         <f t="shared" si="3"/>
         <v>3.6573529411764705E-3</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="7">
         <v>9.52</v>
       </c>
       <c r="H15" s="1">
         <v>-13.7</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="6">
         <f t="shared" si="1"/>
         <v>1.1026834000000001E-2</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="3">
         <v>40.817</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -1614,7 +1622,7 @@
       <c r="N15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="O15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P15" s="1" t="s">
@@ -1623,16 +1631,16 @@
       <c r="Q15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="R15" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U15" s="1" t="s">
+      <c r="T15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U15" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1652,21 +1660,21 @@
       <c r="E16" s="1">
         <v>11.3</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="5">
         <f t="shared" si="3"/>
         <v>3.7180147058823534E-3</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="7">
         <v>11.8</v>
       </c>
       <c r="H16" s="1">
         <v>-21.3</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="6">
         <f t="shared" si="1"/>
         <v>1.0941866000000001E-2</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="3">
         <v>45.7</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -1681,7 +1689,7 @@
       <c r="N16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="O16" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P16" s="1" t="s">
@@ -1690,16 +1698,16 @@
       <c r="Q16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="R16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U16" s="1" t="s">
+      <c r="T16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1719,21 +1727,21 @@
       <c r="E17" s="1">
         <v>-0.3</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="5">
         <f t="shared" si="3"/>
         <v>3.6753676470588238E-3</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="7">
         <v>2</v>
       </c>
       <c r="H17" s="1">
         <v>-26.5</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="6">
         <f t="shared" si="1"/>
         <v>1.0883730000000001E-2</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="3">
         <v>39</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -1748,7 +1756,7 @@
       <c r="N17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P17" s="1" t="s">
@@ -1757,16 +1765,16 @@
       <c r="Q17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="R17" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U17" s="1" t="s">
+      <c r="T17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1786,21 +1794,21 @@
       <c r="E18" s="1">
         <v>1.3</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="5">
         <f t="shared" si="3"/>
         <v>3.6812500000000001E-3</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="7">
         <v>8.8000000000000007</v>
       </c>
       <c r="H18" s="1">
         <v>-9.6</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="6">
         <f t="shared" si="1"/>
         <v>1.1072672E-2</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="3">
         <v>51.9</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -1815,7 +1823,7 @@
       <c r="N18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P18" s="1" t="s">
@@ -1824,16 +1832,16 @@
       <c r="Q18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="R18" s="7" t="s">
         <v>22</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U18" s="1" t="s">
+      <c r="T18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1850,24 +1858,24 @@
       <c r="D19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>-1.2104619999999999</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="5">
         <f t="shared" si="3"/>
         <v>3.6720203602941177E-3</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="7">
         <v>15.721</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>-19.3934</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="6">
         <f t="shared" si="1"/>
         <v>1.0963181788000001E-2</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="3">
         <v>40.442999999999998</v>
       </c>
       <c r="K19" s="1" t="s">
@@ -1882,7 +1890,7 @@
       <c r="N19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="O19" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P19" s="1" t="s">
@@ -1891,16 +1899,16 @@
       <c r="Q19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="1">
+      <c r="R19" s="7">
         <v>35.915999999999997</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U19" s="1">
+      <c r="T19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U19" s="3">
         <v>7.9189999999999996</v>
       </c>
     </row>
@@ -1917,24 +1925,24 @@
       <c r="D20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>-9.9298600000000015</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="5">
         <f t="shared" si="3"/>
         <v>3.63996375E-3</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="7">
         <v>10.523</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>-21.766460000000002</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="6">
         <f t="shared" si="1"/>
         <v>1.0936650977200001E-2</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="3">
         <v>36.094999999999999</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -1949,7 +1957,7 @@
       <c r="N20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="O20" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P20" s="1" t="s">
@@ -1958,16 +1966,16 @@
       <c r="Q20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R20" s="1">
+      <c r="R20" s="7">
         <v>48.081000000000003</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U20" s="1">
+      <c r="T20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20" s="3">
         <v>5.3010000000000002</v>
       </c>
     </row>
@@ -1987,19 +1995,19 @@
       <c r="E21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="1">
+      <c r="F21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="7">
         <v>9.52</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="1">
+      <c r="I21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="3">
         <v>40.817</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -2014,7 +2022,7 @@
       <c r="N21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="O21" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P21" s="1" t="s">
@@ -2023,16 +2031,16 @@
       <c r="Q21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R21" s="1">
+      <c r="R21" s="7">
         <v>43.497999999999998</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U21" s="1">
+      <c r="T21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="3">
         <v>6.1660000000000004</v>
       </c>
     </row>
@@ -2049,24 +2057,24 @@
       <c r="D22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>1.7675399999999999</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="5">
         <f t="shared" si="3"/>
         <v>3.6829688970588231E-3</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="7">
         <v>18.658999999999999</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>-45.725900000000003</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="6">
         <f t="shared" si="1"/>
         <v>1.0668784438000001E-2</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="3">
         <v>32</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -2081,7 +2089,7 @@
       <c r="N22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="O22" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P22" s="1" t="s">
@@ -2090,16 +2098,16 @@
       <c r="Q22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R22" s="1">
+      <c r="R22" s="7">
         <v>42.627000000000002</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U22" s="1">
+      <c r="T22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U22" s="3">
         <v>6.7140000000000004</v>
       </c>
     </row>
@@ -2116,24 +2124,24 @@
       <c r="D23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>-0.94016599999999995</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="5">
         <f t="shared" si="3"/>
         <v>3.6730140955882353E-3</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="7">
         <v>27.082999999999998</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>-9.4759599999999988</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="6">
         <f t="shared" si="1"/>
         <v>1.1074058767200001E-2</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="3">
         <v>46.447000000000003</v>
       </c>
       <c r="K23" s="1" t="s">
@@ -2148,7 +2156,7 @@
       <c r="N23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="O23" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P23" s="1" t="s">
@@ -2157,16 +2165,16 @@
       <c r="Q23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R23" s="1">
+      <c r="R23" s="7">
         <v>20.623999999999999</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U23" s="1">
+      <c r="T23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U23" s="3">
         <v>5.8470000000000004</v>
       </c>
     </row>
@@ -2183,24 +2191,24 @@
       <c r="D24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>-2.3436166666666662</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="5">
         <f t="shared" si="3"/>
         <v>3.6678543504901958E-3</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="7">
         <v>10.678000000000001</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>-13.326050000000002</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="6">
         <f t="shared" si="1"/>
         <v>1.1031014761000001E-2</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="3">
         <v>54.938000000000002</v>
       </c>
       <c r="K24" s="1" t="s">
@@ -2215,7 +2223,7 @@
       <c r="N24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="O24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P24" s="1" t="s">
@@ -2224,16 +2232,16 @@
       <c r="Q24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R24" s="1">
+      <c r="R24" s="7">
         <v>24.393999999999998</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U24" s="1">
+      <c r="T24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U24" s="3">
         <v>9.9890000000000008</v>
       </c>
     </row>
@@ -2250,24 +2258,24 @@
       <c r="D25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>0.35011250000000005</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="5">
         <f t="shared" si="3"/>
         <v>3.6777577665441179E-3</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="7">
         <v>10.678000000000001</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>-13.493425</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="6">
         <f t="shared" si="1"/>
         <v>1.1029143508500001E-2</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="3">
         <v>54.938000000000002</v>
       </c>
       <c r="K25" s="1" t="s">
@@ -2282,7 +2290,7 @@
       <c r="N25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="O25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P25" s="1" t="s">
@@ -2291,16 +2299,16 @@
       <c r="Q25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R25" s="1">
+      <c r="R25" s="7">
         <v>24.393999999999998</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U25" s="1">
+      <c r="T25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U25" s="3">
         <v>9.9890000000000008</v>
       </c>
     </row>
@@ -2317,24 +2325,24 @@
       <c r="D26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>0.78881200000000007</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="5">
         <f t="shared" si="3"/>
         <v>3.6793706323529408E-3</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="7">
         <v>19.163</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>-28.00938</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="6">
         <f t="shared" si="1"/>
         <v>1.0866855131600002E-2</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="3">
         <v>49.295999999999999</v>
       </c>
       <c r="K26" s="1" t="s">
@@ -2349,7 +2357,7 @@
       <c r="N26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="O26" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P26" s="1" t="s">
@@ -2358,16 +2366,16 @@
       <c r="Q26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R26" s="1">
+      <c r="R26" s="7">
         <v>21.888999999999999</v>
       </c>
       <c r="S26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U26" s="1">
+      <c r="T26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26" s="3">
         <v>9.6530000000000005</v>
       </c>
     </row>
@@ -2384,24 +2392,24 @@
       <c r="D27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>-1.5775499999999998</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="5">
         <f t="shared" si="3"/>
         <v>3.6706707720588231E-3</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="7">
         <v>9.3872</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>-33.4637125</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="6">
         <f>$I$2*(H27/1000+1)</f>
         <v>1.0805875694250001E-2</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="3">
         <v>40.247300000000003</v>
       </c>
       <c r="K27" s="1" t="s">
@@ -2416,7 +2424,7 @@
       <c r="N27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="O27" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P27" s="1" t="s">
@@ -2425,16 +2433,16 @@
       <c r="Q27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R27" s="1">
+      <c r="R27" s="7">
         <v>21.4453</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U27" s="1">
+      <c r="T27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U27" s="3">
         <v>7.4306000000000001</v>
       </c>
     </row>
@@ -2451,24 +2459,24 @@
       <c r="D28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>14.163140000000002</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="5">
         <f t="shared" si="3"/>
         <v>3.7285409558823527E-3</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="7">
         <v>10.678000000000001</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>-27.616899999999998</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="6">
         <f t="shared" si="1"/>
         <v>1.0871243058000002E-2</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="3">
         <v>54.938000000000002</v>
       </c>
       <c r="K28" s="1" t="s">
@@ -2483,7 +2491,7 @@
       <c r="N28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="O28" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P28" s="1" t="s">
@@ -2492,16 +2500,16 @@
       <c r="Q28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R28" s="1">
+      <c r="R28" s="7">
         <v>24.393999999999998</v>
       </c>
       <c r="S28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U28" s="1">
+      <c r="T28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" s="3">
         <v>9.9890000000000008</v>
       </c>
     </row>
@@ -2518,24 +2526,24 @@
       <c r="D29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>2.1924000000000001</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="5">
         <f t="shared" si="3"/>
         <v>3.6845308823529412E-3</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="7">
         <v>8.4792000000000005</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>-11.7986</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="6">
         <f t="shared" si="1"/>
         <v>1.1048091652E-2</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="3">
         <v>65.437899999999999</v>
       </c>
       <c r="K29" s="1" t="s">
@@ -2550,7 +2558,7 @@
       <c r="N29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="O29" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P29" s="1" t="s">
@@ -2559,16 +2567,16 @@
       <c r="Q29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R29" s="1">
+      <c r="R29" s="7">
         <v>19.370999999999999</v>
       </c>
       <c r="S29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U29" s="1">
+      <c r="T29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U29" s="3">
         <v>6.7119</v>
       </c>
     </row>
@@ -2585,24 +2593,24 @@
       <c r="D30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>1.5505800000000001</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="5">
         <f t="shared" si="3"/>
         <v>3.68217125E-3</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="7">
         <v>12.165900000000001</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <v>-11.291300000000001</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="6">
         <f t="shared" si="1"/>
         <v>1.1053763266000001E-2</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="3">
         <v>52.161299999999997</v>
       </c>
       <c r="K30" s="1" t="s">
@@ -2617,7 +2625,7 @@
       <c r="N30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="O30" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P30" s="1" t="s">
@@ -2626,16 +2634,16 @@
       <c r="Q30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R30" s="1">
+      <c r="R30" s="7">
         <v>27.793500000000002</v>
       </c>
       <c r="S30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U30" s="1">
+      <c r="T30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U30" s="3">
         <v>7.8792999999999997</v>
       </c>
     </row>
@@ -2652,24 +2660,24 @@
       <c r="D31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>-1.7516750000000001</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="5">
         <f t="shared" si="3"/>
         <v>3.6700306066176471E-3</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="7">
         <v>13.327999999999999</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <v>-7.8926999999999996</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31" s="6">
         <f t="shared" si="1"/>
         <v>1.1091759614000002E-2</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="3">
         <v>34.286099999999998</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -2684,7 +2692,7 @@
       <c r="N31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="O31" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P31" s="1" t="s">
@@ -2693,16 +2701,16 @@
       <c r="Q31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R31" s="1">
+      <c r="R31" s="7">
         <v>45.6723</v>
       </c>
       <c r="S31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U31" s="1">
+      <c r="T31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U31" s="3">
         <v>6.7137000000000002</v>
       </c>
     </row>
@@ -2719,24 +2727,24 @@
       <c r="D32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>4.8876249999999996E-2</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="5">
         <f t="shared" si="3"/>
         <v>3.6766502803308823E-3</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="7">
         <v>11.758599999999999</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>-11.36345</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32" s="6">
         <f t="shared" si="1"/>
         <v>1.1052956629000001E-2</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="3">
         <v>40.331699999999998</v>
       </c>
       <c r="K32" s="1" t="s">
@@ -2751,7 +2759,7 @@
       <c r="N32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="O32" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P32" s="1" t="s">
@@ -2760,16 +2768,16 @@
       <c r="Q32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R32" s="1">
+      <c r="R32" s="7">
         <v>40.2943</v>
       </c>
       <c r="S32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U32" s="1">
+      <c r="T32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U32" s="3">
         <v>7.6154000000000002</v>
       </c>
     </row>
@@ -2786,24 +2794,24 @@
       <c r="D33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>3.2947499999999996</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="5">
         <f t="shared" si="3"/>
         <v>3.6885836397058825E-3</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="7">
         <v>7.7305000000000001</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>-22.567500000000003</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33" s="6">
         <f t="shared" si="1"/>
         <v>1.0927695350000001E-2</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33" s="3">
         <v>59.659599999999998</v>
       </c>
       <c r="K33" s="1" t="s">
@@ -2818,7 +2826,7 @@
       <c r="N33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="O33" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P33" s="1" t="s">
@@ -2827,16 +2835,16 @@
       <c r="Q33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R33" s="1">
+      <c r="R33" s="7">
         <v>26.4907</v>
       </c>
       <c r="S33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U33" s="1">
+      <c r="T33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U33" s="3">
         <v>6.1192000000000002</v>
       </c>
     </row>
@@ -2853,24 +2861,24 @@
       <c r="D34" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>0.36097499999999999</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="5">
         <f t="shared" si="3"/>
         <v>3.6777977022058824E-3</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="7">
         <v>11.9566</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>-12.276412499999999</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="6">
         <f t="shared" si="1"/>
         <v>1.1042749708250001E-2</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="3">
         <v>51.2637</v>
       </c>
       <c r="K34" s="1" t="s">
@@ -2885,7 +2893,7 @@
       <c r="N34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="O34" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P34" s="1" t="s">
@@ -2894,16 +2902,16 @@
       <c r="Q34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R34" s="1">
+      <c r="R34" s="7">
         <v>27.315200000000001</v>
       </c>
       <c r="S34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U34" s="1">
+      <c r="T34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U34" s="3">
         <v>9.4644999999999992</v>
       </c>
     </row>
@@ -2929,10 +2937,10 @@
       <c r="G35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="2">
         <v>-30.561609999999995</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35" s="6">
         <f t="shared" si="1"/>
         <v>1.08383212002E-2</v>
       </c>
@@ -2951,7 +2959,7 @@
       <c r="N35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="O35" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P35" s="1" t="s">
@@ -2966,7 +2974,7 @@
       <c r="S35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T35" s="1" t="s">
+      <c r="T35" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U35" s="1" t="s">
@@ -2995,10 +3003,10 @@
       <c r="G36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="2">
         <v>-29.274849999999997</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="6">
         <f t="shared" si="1"/>
         <v>1.0852707177000001E-2</v>
       </c>
@@ -3017,7 +3025,7 @@
       <c r="N36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="O36" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P36" s="1" t="s">
@@ -3032,7 +3040,7 @@
       <c r="S36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T36" s="1" t="s">
+      <c r="T36" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U36" s="1" t="s">
@@ -3061,10 +3069,10 @@
       <c r="G37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="2">
         <v>-28.428689999999996</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="6">
         <f t="shared" si="1"/>
         <v>1.0862167245800001E-2</v>
       </c>
@@ -3083,7 +3091,7 @@
       <c r="N37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="O37" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P37" s="1" t="s">
@@ -3098,7 +3106,7 @@
       <c r="S37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T37" s="1" t="s">
+      <c r="T37" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U37" s="1" t="s">
@@ -3127,10 +3135,10 @@
       <c r="G38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="2">
         <v>-26.576659999999997</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="6">
         <f t="shared" si="1"/>
         <v>1.08828729412E-2</v>
       </c>
@@ -3149,7 +3157,7 @@
       <c r="N38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="O38" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P38" s="1" t="s">
@@ -3164,7 +3172,7 @@
       <c r="S38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T38" s="1" t="s">
+      <c r="T38" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U38" s="1" t="s">
@@ -3196,7 +3204,7 @@
       <c r="H39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I39" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J39" s="1" t="s">
@@ -3214,7 +3222,7 @@
       <c r="N39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="O39" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P39" s="1" t="s">
@@ -3229,7 +3237,7 @@
       <c r="S39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T39" s="1" t="s">
+      <c r="T39" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U39" s="1" t="s">
@@ -3258,10 +3266,10 @@
       <c r="G40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="2">
         <v>-29.848129999999998</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="6">
         <f t="shared" si="1"/>
         <v>1.0846297906600001E-2</v>
       </c>
@@ -3280,7 +3288,7 @@
       <c r="N40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="O40" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P40" s="1" t="s">
@@ -3295,7 +3303,7 @@
       <c r="S40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T40" s="1" t="s">
+      <c r="T40" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U40" s="1" t="s">
@@ -3324,10 +3332,10 @@
       <c r="G41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
         <v>-28.465210000000003</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="6">
         <f t="shared" si="1"/>
         <v>1.08617589522E-2</v>
       </c>
@@ -3346,7 +3354,7 @@
       <c r="N41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O41" s="1" t="s">
+      <c r="O41" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P41" s="1" t="s">
@@ -3361,7 +3369,7 @@
       <c r="S41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T41" s="1" t="s">
+      <c r="T41" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U41" s="1" t="s">
@@ -3390,10 +3398,10 @@
       <c r="G42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
         <v>-31.612680000000001</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I42" s="6">
         <f t="shared" si="1"/>
         <v>1.0826570237599999E-2</v>
       </c>
@@ -3412,7 +3420,7 @@
       <c r="N42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O42" s="1" t="s">
+      <c r="O42" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P42" s="1" t="s">
@@ -3427,7 +3435,7 @@
       <c r="S42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T42" s="1" t="s">
+      <c r="T42" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U42" s="1" t="s">
@@ -3456,10 +3464,10 @@
       <c r="G43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
         <v>-12.954180000000003</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I43" s="6">
         <f t="shared" si="1"/>
         <v>1.1035172267600001E-2</v>
       </c>
@@ -3478,7 +3486,7 @@
       <c r="N43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O43" s="1" t="s">
+      <c r="O43" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P43" s="1" t="s">
@@ -3493,7 +3501,7 @@
       <c r="S43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T43" s="1" t="s">
+      <c r="T43" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U43" s="1" t="s">
@@ -3522,10 +3530,10 @@
       <c r="G44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="2">
         <v>-11.805139999999998</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I44" s="6">
         <f t="shared" si="1"/>
         <v>1.1048018534800001E-2</v>
       </c>
@@ -3544,7 +3552,7 @@
       <c r="N44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O44" s="1" t="s">
+      <c r="O44" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P44" s="1" t="s">
@@ -3559,7 +3567,7 @@
       <c r="S44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T44" s="1" t="s">
+      <c r="T44" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U44" s="1" t="s">
@@ -3588,10 +3596,10 @@
       <c r="G45" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I45" s="3" t="s">
+      <c r="H45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J45" s="1" t="s">
@@ -3609,7 +3617,7 @@
       <c r="N45" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O45" s="1" t="s">
+      <c r="O45" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P45" s="1" t="s">
@@ -3624,7 +3632,7 @@
       <c r="S45" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T45" s="1" t="s">
+      <c r="T45" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U45" s="1" t="s">
@@ -3653,10 +3661,10 @@
       <c r="G46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I46" s="3" t="s">
+      <c r="H46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J46" s="1" t="s">
@@ -3674,7 +3682,7 @@
       <c r="N46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O46" s="1" t="s">
+      <c r="O46" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P46" s="1" t="s">
@@ -3689,7 +3697,7 @@
       <c r="S46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="T46" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U46" s="1" t="s">
@@ -3718,10 +3726,10 @@
       <c r="G47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I47" s="3" t="s">
+      <c r="H47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J47" s="1" t="s">
@@ -3739,7 +3747,7 @@
       <c r="N47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O47" s="1" t="s">
+      <c r="O47" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P47" s="1" t="s">
@@ -3754,7 +3762,7 @@
       <c r="S47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T47" s="1" t="s">
+      <c r="T47" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U47" s="1" t="s">
@@ -3783,10 +3791,10 @@
       <c r="G48" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="2">
         <v>-17.7639</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I48" s="6">
         <f t="shared" si="1"/>
         <v>1.0981399598E-2</v>
       </c>
@@ -3805,7 +3813,7 @@
       <c r="N48" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="O48" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P48" s="1" t="s">
@@ -3820,7 +3828,7 @@
       <c r="S48" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T48" s="1" t="s">
+      <c r="T48" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U48" s="1" t="s">
@@ -3849,10 +3857,10 @@
       <c r="G49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="2">
         <v>-30.688419999999997</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49" s="6">
         <f t="shared" si="1"/>
         <v>1.08369034644E-2</v>
       </c>
@@ -3871,7 +3879,7 @@
       <c r="N49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O49" s="1" t="s">
+      <c r="O49" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P49" s="1" t="s">
@@ -3886,7 +3894,7 @@
       <c r="S49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T49" s="1" t="s">
+      <c r="T49" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U49" s="1" t="s">
@@ -3915,10 +3923,10 @@
       <c r="G50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="2">
         <v>-29.979620000000004</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50" s="6">
         <f t="shared" si="1"/>
         <v>1.0844827848400001E-2</v>
       </c>
@@ -3937,7 +3945,7 @@
       <c r="N50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O50" s="1" t="s">
+      <c r="O50" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P50" s="1" t="s">
@@ -3952,7 +3960,7 @@
       <c r="S50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T50" s="1" t="s">
+      <c r="T50" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U50" s="1" t="s">
@@ -3981,10 +3989,10 @@
       <c r="G51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="2">
         <v>-29.804650000000002</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I51" s="6">
         <f t="shared" si="1"/>
         <v>1.0846784013E-2</v>
       </c>
@@ -4003,7 +4011,7 @@
       <c r="N51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O51" s="1" t="s">
+      <c r="O51" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P51" s="1" t="s">
@@ -4018,7 +4026,7 @@
       <c r="S51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T51" s="1" t="s">
+      <c r="T51" s="5" t="s">
         <v>22</v>
       </c>
       <c r="U51" s="1" t="s">
@@ -4050,7 +4058,7 @@
       <c r="H52" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="I52" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J52" s="1" t="s">
@@ -4068,7 +4076,7 @@
       <c r="N52" s="1">
         <v>0</v>
       </c>
-      <c r="O52" s="1">
+      <c r="O52" s="5">
         <f>$O$4*(N52/1000+1)</f>
         <v>2.0051711041251551E-3</v>
       </c>
@@ -4084,7 +4092,7 @@
       <c r="S52" s="1">
         <v>0.65</v>
       </c>
-      <c r="T52" s="1">
+      <c r="T52" s="5">
         <f>$T$4*(S52/1000+1)</f>
         <v>1.558655054938256E-4</v>
       </c>
@@ -4117,7 +4125,7 @@
       <c r="H53" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="I53" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J53" s="1" t="s">
@@ -4135,7 +4143,7 @@
       <c r="N53" s="1">
         <v>-10.55</v>
       </c>
-      <c r="O53" s="1">
+      <c r="O53" s="5">
         <f>$O$4*(N53/1000+1)</f>
         <v>1.9840165489766349E-3</v>
       </c>
@@ -4151,7 +4159,7 @@
       <c r="S53" s="1">
         <v>-75.63</v>
       </c>
-      <c r="T53" s="1">
+      <c r="T53" s="5">
         <f>$T$4*(S53/1000+1)</f>
         <v>1.4398380783823273E-4</v>
       </c>
@@ -4184,7 +4192,7 @@
       <c r="H54" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="I54" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J54" s="1" t="s">
@@ -4202,7 +4210,7 @@
       <c r="N54" s="1">
         <v>-20.010000000000002</v>
       </c>
-      <c r="O54" s="1">
+      <c r="O54" s="5">
         <f>$O$4*(N54/1000+1)</f>
         <v>1.9650476303316108E-3</v>
       </c>
@@ -4218,7 +4226,7 @@
       <c r="S54" s="1">
         <v>-156.87</v>
       </c>
-      <c r="T54" s="1">
+      <c r="T54" s="5">
         <f>$T$4*(S54/1000+1)</f>
         <v>1.3132951945936058E-4</v>
       </c>

</xml_diff>